<commit_message>
Add Lobby UI & Wave System & HP bar
</commit_message>
<xml_diff>
--- a/Assets/7.DataBase/DataBase.xlsx
+++ b/Assets/7.DataBase/DataBase.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\82108\Documents\GitHub\Com2us_Mentoring\Assets\7.DataBase\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sojun\OneDrive\문서\GitHub\Com2us_Mentoring\Assets\7.DataBase\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DDD1AB8-0AE5-4B37-BB16-97FFDC79CCCE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B16A15FB-55A0-48B2-A365-3DBAB8801715}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{FCB4753B-0ECC-4CCA-9BCB-76EE9CDBFC0F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="3" xr2:uid="{FCB4753B-0ECC-4CCA-9BCB-76EE9CDBFC0F}"/>
   </bookViews>
   <sheets>
     <sheet name="TowerEntities" sheetId="1" r:id="rId1"/>
@@ -422,7 +422,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E0944A6F-73A8-4D73-A68F-C8EA68B1FE23}">
   <dimension ref="A1:D21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
@@ -1232,8 +1232,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{24217607-DA08-4799-AF0A-FAA062684C5B}">
   <dimension ref="A1:C21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G25" sqref="G25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M18" sqref="M18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1257,7 +1257,7 @@
         <v>1</v>
       </c>
       <c r="C2">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
@@ -1268,7 +1268,7 @@
         <v>0.95</v>
       </c>
       <c r="C3">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
@@ -1279,7 +1279,7 @@
         <v>0.9</v>
       </c>
       <c r="C4">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
@@ -1290,7 +1290,7 @@
         <v>0.85</v>
       </c>
       <c r="C5">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
@@ -1301,7 +1301,7 @@
         <v>0.8</v>
       </c>
       <c r="C6">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
@@ -1312,7 +1312,7 @@
         <v>0.75</v>
       </c>
       <c r="C7">
-        <v>6</v>
+        <v>3.6</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
@@ -1323,7 +1323,7 @@
         <v>0.7</v>
       </c>
       <c r="C8">
-        <v>6</v>
+        <v>3.6</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
@@ -1334,7 +1334,7 @@
         <v>0.65</v>
       </c>
       <c r="C9">
-        <v>6</v>
+        <v>3.6</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
@@ -1345,7 +1345,7 @@
         <v>0.6</v>
       </c>
       <c r="C10">
-        <v>6</v>
+        <v>3.6</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
@@ -1356,7 +1356,7 @@
         <v>0.55000000000000004</v>
       </c>
       <c r="C11">
-        <v>6</v>
+        <v>3.6</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
@@ -1367,7 +1367,7 @@
         <v>0.5</v>
       </c>
       <c r="C12">
-        <v>7</v>
+        <v>4.3</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
@@ -1378,7 +1378,7 @@
         <v>0.45</v>
       </c>
       <c r="C13">
-        <v>7</v>
+        <v>4.3</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
@@ -1389,7 +1389,7 @@
         <v>0.4</v>
       </c>
       <c r="C14">
-        <v>7</v>
+        <v>4.3</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
@@ -1400,7 +1400,7 @@
         <v>0.35</v>
       </c>
       <c r="C15">
-        <v>7</v>
+        <v>4.3</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
@@ -1411,7 +1411,7 @@
         <v>0.3</v>
       </c>
       <c r="C16">
-        <v>7</v>
+        <v>4.3</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
@@ -1422,7 +1422,7 @@
         <v>0.25</v>
       </c>
       <c r="C17">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
@@ -1433,7 +1433,7 @@
         <v>0.2</v>
       </c>
       <c r="C18">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
@@ -1444,7 +1444,7 @@
         <v>0.15</v>
       </c>
       <c r="C19">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
@@ -1455,7 +1455,7 @@
         <v>0.1</v>
       </c>
       <c r="C20">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
@@ -1466,7 +1466,7 @@
         <v>0.05</v>
       </c>
       <c r="C21">
-        <v>9</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>